<commit_message>
nuevo page + test05
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataDriven.xlsx
+++ b/src/main/resources/Data/DataDriven.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matias.rojas\IdeaProjects\PageObjectModel_Curso_Selenium\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01CB304-0FE4-429F-961C-EC2DB5F4858D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1636887B-5FBB-4AF0-8FB9-9209D58E9115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{C46FAF6A-F493-4035-8392-1F2F68894BAB}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
-  <si>
-    <t>ATC06</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>ATC07</t>
   </si>
@@ -81,13 +78,10 @@
     <t>Rojas651</t>
   </si>
   <si>
-    <t>ATC05_PagarCuenta</t>
-  </si>
-  <si>
-    <t>126554850</t>
-  </si>
-  <si>
-    <t>Directv</t>
+    <t>ATC05_descargarCartola6meses</t>
+  </si>
+  <si>
+    <t>ATC06_descargarCartolaLuz</t>
   </si>
 </sst>
 </file>
@@ -453,12 +447,12 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -468,99 +462,102 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agrego nuevo test06
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/DataDriven.xlsx
+++ b/src/main/resources/Data/DataDriven.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matias.rojas\IdeaProjects\PageObjectModel_Curso_Selenium\src\main\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1636887B-5FBB-4AF0-8FB9-9209D58E9115}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBC7D78-BD07-4D90-AA15-77A2296D3152}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{C46FAF6A-F493-4035-8392-1F2F68894BAB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>ATC07</t>
   </si>
@@ -51,9 +51,6 @@
     <t>id_cuenta</t>
   </si>
   <si>
-    <t>cuenta</t>
-  </si>
-  <si>
     <t>empresa</t>
   </si>
   <si>
@@ -82,6 +79,15 @@
   </si>
   <si>
     <t>ATC06_descargarCartolaLuz</t>
+  </si>
+  <si>
+    <t>servicio</t>
+  </si>
+  <si>
+    <t>Luz</t>
+  </si>
+  <si>
+    <t>CGE</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,16 +468,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
@@ -485,10 +491,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -496,13 +502,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -510,13 +516,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G4" s="3"/>
     </row>
@@ -525,29 +531,35 @@
         <v>5</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>